<commit_message>
Feat: txt_debug and reload button on UI
Feat: SD card detection
Unfinished: Reload SD card properly
</commit_message>
<xml_diff>
--- a/hw02_photo_frame/TouchGFX/assets/texts/texts.xlsx
+++ b/hw02_photo_frame/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9429" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9987" uniqueCount="146">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2367,8 +2367,40 @@
         <v>145</v>
       </c>
     </row>
-    <row r="31"/>
-    <row r="32"/>
+    <row r="31">
+      <c r="B31" t="s">
+        <v>129</v>
+      </c>
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="s">
+        <v>131</v>
+      </c>
+      <c r="C32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" t="s">
+        <v>102</v>
+      </c>
+    </row>
     <row r="33"/>
     <row r="34"/>
     <row r="35"/>

</xml_diff>

<commit_message>
misc: UI: Add screen_initial, display loading message
functions will be implemented next commit.
This commit has no function but just display screen_initial.
</commit_message>
<xml_diff>
--- a/hw02_photo_frame/TouchGFX/assets/texts/texts.xlsx
+++ b/hw02_photo_frame/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9987" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11733" uniqueCount="154">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -457,6 +457,62 @@
   </si>
   <si>
     <t xml:space="preserve">Duration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">數位相框
+Digital Frame
+Loading Bitmaps...
+Please wait for a moment.
+載入中</t>
+  </si>
+  <si>
+    <t xml:space="preserve">數位相框
+Digital Frame
+Loading Bitmaps...
+Please wait for a moment.
+載入中</t>
+  </si>
+  <si>
+    <t xml:space="preserve">數位相框
+Digital Frame
+Loading Bitmaps...
+Please wait for a moment.
+載入中...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">數位相框
+Digital Frame
+Loading Bitmaps...
+Please wait for a moment.
+載入中...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">數位相框
+Digital Frame
+Loading Bitmaps...
+Please wait for a moment.
+載入中...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">數位相框
+Digital Frame
+Loading Bitmaps...
+Please wait for a moment.
+載入中...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">數位相框
+Digital Frame
+Loading Bitmaps...
+Please wait for a moment.
+載入中...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">數位相框
+Digital Frame
+Loading Bitmaps...
+Please wait for a moment.
+載入中...</t>
   </si>
 </sst>
 </file>
@@ -2401,7 +2457,23 @@
         <v>102</v>
       </c>
     </row>
-    <row r="33"/>
+    <row r="33">
+      <c r="B33" t="s">
+        <v>133</v>
+      </c>
+      <c r="C33" t="s">
+        <v>116</v>
+      </c>
+      <c r="D33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" t="s">
+        <v>153</v>
+      </c>
+    </row>
     <row r="34"/>
     <row r="35"/>
     <row r="36"/>

</xml_diff>